<commit_message>
update to measurements file
</commit_message>
<xml_diff>
--- a/data/raw/measurements/20200205_measurements.xlsx
+++ b/data/raw/measurements/20200205_measurements.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">200207_0_3</t>
   </si>
   <si>
-    <t xml:space="preserve">200207_2_7</t>
+    <t xml:space="preserve">200206_2_7</t>
   </si>
   <si>
     <t xml:space="preserve">200207_0_7</t>
@@ -180,7 +180,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>